<commit_message>
Fixed assembly picklist creation app
</commit_message>
<xml_diff>
--- a/frontend/static/file_examples/create_assembly_picklists/example_echo_plate.xlsx
+++ b/frontend/static/file_examples/create_assembly_picklists/example_echo_plate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="content" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,10 +27,10 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">conn a-c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conn w-x</t>
+    <t xml:space="preserve">conn_a-c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conn_w-x</t>
   </si>
   <si>
     <t xml:space="preserve">p19_mtagbfp2</t>
@@ -48,10 +48,10 @@
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">conn b-e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conn w-y</t>
+    <t xml:space="preserve">conn_b-e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conn_w-y</t>
   </si>
   <si>
     <t xml:space="preserve">p19_tet-on-3g</t>
@@ -69,10 +69,10 @@
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">conn b-l</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conn w-z</t>
+    <t xml:space="preserve">conn_b-l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conn_w-z</t>
   </si>
   <si>
     <t xml:space="preserve">p1_5'-itr-pb</t>
@@ -90,10 +90,10 @@
     <t xml:space="preserve">D</t>
   </si>
   <si>
-    <t xml:space="preserve">conn d-e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conn y-z</t>
+    <t xml:space="preserve">conn_d-e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conn_y-z</t>
   </si>
   <si>
     <t xml:space="preserve">p1_5'ha-haavs1</t>
@@ -111,7 +111,7 @@
     <t xml:space="preserve">E</t>
   </si>
   <si>
-    <t xml:space="preserve">conn d-f</t>
+    <t xml:space="preserve">conn_d-f</t>
   </si>
   <si>
     <t xml:space="preserve">hc_amp_ccdb</t>
@@ -132,7 +132,7 @@
     <t xml:space="preserve">F</t>
   </si>
   <si>
-    <t xml:space="preserve">conn h-ha</t>
+    <t xml:space="preserve">conn_h-ha</t>
   </si>
   <si>
     <t xml:space="preserve">no_clone</t>
@@ -153,7 +153,7 @@
     <t xml:space="preserve">G</t>
   </si>
   <si>
-    <t xml:space="preserve">conn h-j</t>
+    <t xml:space="preserve">conn_h-j</t>
   </si>
   <si>
     <t xml:space="preserve">p10_tet-aptazyme</t>
@@ -168,13 +168,13 @@
     <t xml:space="preserve">p7_l7ae-weiss</t>
   </si>
   <si>
-    <t xml:space="preserve">p9_firefly luciferase</t>
+    <t xml:space="preserve">p9_firefly_luciferase</t>
   </si>
   <si>
     <t xml:space="preserve">H</t>
   </si>
   <si>
-    <t xml:space="preserve">conn h-k</t>
+    <t xml:space="preserve">conn_h-k</t>
   </si>
   <si>
     <t xml:space="preserve">p11_sv40polya</t>
@@ -195,7 +195,7 @@
     <t xml:space="preserve">I</t>
   </si>
   <si>
-    <t xml:space="preserve">conn j-k</t>
+    <t xml:space="preserve">conn_j-k</t>
   </si>
   <si>
     <t xml:space="preserve">p14_cmvp</t>
@@ -216,7 +216,7 @@
     <t xml:space="preserve">J</t>
   </si>
   <si>
-    <t xml:space="preserve">conn l-n</t>
+    <t xml:space="preserve">conn_l-n</t>
   </si>
   <si>
     <t xml:space="preserve">p14_sv40p</t>
@@ -237,7 +237,7 @@
     <t xml:space="preserve">K</t>
   </si>
   <si>
-    <t xml:space="preserve">conn l-r</t>
+    <t xml:space="preserve">conn_l-r</t>
   </si>
   <si>
     <t xml:space="preserve">p15_puror</t>
@@ -258,7 +258,7 @@
     <t xml:space="preserve">L</t>
   </si>
   <si>
-    <t xml:space="preserve">conn l-w</t>
+    <t xml:space="preserve">conn_l-w</t>
   </si>
   <si>
     <t xml:space="preserve">p16_bghpolya</t>
@@ -279,7 +279,7 @@
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">conn l-y</t>
+    <t xml:space="preserve">conn_l-y</t>
   </si>
   <si>
     <t xml:space="preserve">p18_cmvp</t>
@@ -297,7 +297,7 @@
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">conn q-r</t>
+    <t xml:space="preserve">conn_q-r</t>
   </si>
   <si>
     <t xml:space="preserve">p18_ef1ap</t>
@@ -315,7 +315,7 @@
     <t xml:space="preserve">O</t>
   </si>
   <si>
-    <t xml:space="preserve">conn r-w</t>
+    <t xml:space="preserve">conn_r-w</t>
   </si>
   <si>
     <t xml:space="preserve">p19_mneogreen</t>
@@ -336,7 +336,7 @@
     <t xml:space="preserve">P</t>
   </si>
   <si>
-    <t xml:space="preserve">conn t-v</t>
+    <t xml:space="preserve">conn_t-v</t>
   </si>
   <si>
     <t xml:space="preserve">p19_mruby2</t>
@@ -476,8 +476,8 @@
   </sheetPr>
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y17" activeCellId="0" sqref="Y17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -485,7 +485,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,7 +811,7 @@
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -1308,7 +1311,7 @@
   </sheetPr>
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Y16" activeCellId="0" sqref="Y16"/>
     </sheetView>
   </sheetViews>
@@ -2642,7 +2645,7 @@
   </sheetPr>
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="X21" activeCellId="0" sqref="X21"/>
     </sheetView>
   </sheetViews>

</xml_diff>